<commit_message>
handled all errors during inserting data to mysql
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\cms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082CE694-A061-4388-AAAE-1144E5B0AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E83CDCD-5956-4210-8BA6-77213706FF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{E89AEF72-467A-46A4-ACB1-BD3505564FF9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Download folder</t>
   </si>
@@ -141,24 +141,12 @@
     <t>DB tables mapping</t>
   </si>
   <si>
-    <t>HOSPC14_COST_REPORT_STATUS_COUNTS.CSV</t>
-  </si>
-  <si>
-    <t>cost_report_status_counts</t>
-  </si>
-  <si>
     <t>providers</t>
   </si>
   <si>
     <t>HOSPC14_PRVDR_ID_INFO.csv</t>
   </si>
   <si>
-    <t>record_counts</t>
-  </si>
-  <si>
-    <t>HOSPC14_RECORD_COUNTS.csv</t>
-  </si>
-  <si>
     <t>Download folder path type</t>
   </si>
   <si>
@@ -168,19 +156,31 @@
     <t>Downloads</t>
   </si>
   <si>
-    <t>RPT_REC_NUM;PRVDR_CTRL_TYPE_CD;PRVDR_NUM;NPI;RPT_STUS_CD;FY_BGN_DT;FY_END_DT;PROC_DT;INITL_RPT_SW;LAST_RPT_SW;TRNSMTL_NUM;FI_NUM;ADR_VNDR_CD;FI_CREAT_DT;UTIL_CD;NPR_DT;SPEC_IND;FI_RCPT_DT</t>
-  </si>
-  <si>
     <t>DB columns</t>
   </si>
   <si>
     <t>Default headers</t>
   </si>
   <si>
-    <t>RPT_REC_NUM;WKSHT_CD;LINE_NUM;CLMN_NUM;ALPHNMRC_ITM_TXT</t>
-  </si>
-  <si>
-    <t>RPT_REC_NUM;WKSHT_CD;LINE_NUM;CLMN_NUM;ITM_VAL_NUM</t>
+    <t>RPT_REC_NUM:numeric;WKSHT_CD;LINE_NUM;CLMN_NUM;ALPHNMRC_ITM_TXT</t>
+  </si>
+  <si>
+    <t>Default date format</t>
+  </si>
+  <si>
+    <t>Default number format</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>RPT_REC_NUM:numeric;WKSHT_CD;LINE_NUM;CLMN_NUM;ITM_VAL_NUM:numeric:float</t>
+  </si>
+  <si>
+    <t>RPT_REC_NUM:numeric;PRVDR_CTRL_TYPE_CD;PRVDR_NUM;NPI:numeric:integer;RPT_STUS_CD;FY_BGN_DT:datetime:;FY_END_DT:datetime;PROC_DT:datetime;INITL_RPT_SW;LAST_RPT_SW;TRNSMTL_NUM;FI_NUM;ADR_VNDR_CD;FI_CREAT_DT:datetime;UTIL_CD;NPR_DT:datetime;SPEC_IND;FI_RCPT_DT:datetime</t>
+  </si>
+  <si>
+    <t>%m/%d/%Y</t>
   </si>
 </sst>
 </file>
@@ -335,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -417,6 +417,28 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -454,7 +476,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="3" fillId="10" borderId="1" xfId="15">
       <protection locked="0"/>
@@ -483,6 +505,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="20" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="10" borderId="8" xfId="15" applyBorder="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="10" borderId="7" xfId="15" applyBorder="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -749,8 +777,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FDF0A75-F81B-4CED-8D61-87E14E7DE396}" name="Parameters" displayName="Parameters" ref="B3:C9" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12" headerRowCellStyle="Шапка_справочник" dataCellStyle="Справочник_данные">
-  <autoFilter ref="B3:C9" xr:uid="{6FDF0A75-F81B-4CED-8D61-87E14E7DE396}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6FDF0A75-F81B-4CED-8D61-87E14E7DE396}" name="Parameters" displayName="Parameters" ref="B3:C11" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12" headerRowCellStyle="Шапка_справочник" dataCellStyle="Справочник_данные">
+  <autoFilter ref="B3:C11" xr:uid="{6FDF0A75-F81B-4CED-8D61-87E14E7DE396}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{54BB5CED-4F13-431D-9F31-1BE601F4ED1F}" name="Parameter" dataDxfId="11" dataCellStyle="Справочник_данные"/>
     <tableColumn id="2" xr3:uid="{0FC4D1C5-0363-4F8F-B5F7-65172C05BBC6}" name="Value" dataDxfId="10" dataCellStyle="Справочник_данные"/>
@@ -770,8 +798,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F2EFE16-214D-4348-BEF8-975642B9A3BB}" name="Mappings" displayName="Mappings" ref="G3:J12" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4" headerRowCellStyle="Шапка_справочник" dataCellStyle="Справочник_данные">
-  <autoFilter ref="G3:J12" xr:uid="{8F2EFE16-214D-4348-BEF8-975642B9A3BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F2EFE16-214D-4348-BEF8-975642B9A3BB}" name="Mappings" displayName="Mappings" ref="G3:J10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4" headerRowCellStyle="Шапка_справочник" dataCellStyle="Справочник_данные">
+  <autoFilter ref="G3:J10" xr:uid="{8F2EFE16-214D-4348-BEF8-975642B9A3BB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AFBB63CD-AB05-4E64-9580-DC476A9E2342}" name="DB table" dataDxfId="3" dataCellStyle="Справочник_данные"/>
     <tableColumn id="2" xr3:uid="{6EB8F766-1D92-4659-AE9F-B678C92DF820}" name="Part of file name" dataDxfId="2" dataCellStyle="Справочник_данные"/>
@@ -1079,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF7D921-30C3-488A-B359-12D8C7E82A3F}">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,10 +1156,10 @@
         <v>18</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -1154,7 +1182,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -1177,7 +1205,7 @@
         <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -1185,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -1200,15 +1228,15 @@
         <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>26</v>
@@ -1258,11 +1286,17 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="G10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>2</v>
@@ -1270,32 +1304,16 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3"/>
+      <c r="B11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8 I4:I12" xr:uid="{B84025B2-0BB6-4DFF-B9A7-62018F24049C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8 I4:I10" xr:uid="{B84025B2-0BB6-4DFF-B9A7-62018F24049C}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{75D249D4-DDDF-4F35-AACB-7F3E20D37076}">

</xml_diff>

<commit_message>
fixed column and lne numbers
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\cms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E83CDCD-5956-4210-8BA6-77213706FF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9E6ED7-BA36-4251-8F1B-D2E6CC1C2C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{E89AEF72-467A-46A4-ACB1-BD3505564FF9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Download folder</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>%m/%d/%Y</t>
+  </si>
+  <si>
+    <t>var * {RPT_REC_NUM: int64, WKSHT_CD: string, LINE_NUM: string, CLMN_NUM: string, ALPHNMRC_ITM_TXT: string}</t>
+  </si>
+  <si>
+    <t>var * {RPT_REC_NUM: int64, WKSHT_CD: string, LINE_NUM: string, CLMN_NUM: string, ITM_VAL_NUM: float64}</t>
+  </si>
+  <si>
+    <t>var * {RPT_REC_NUM: int64, PRVDR_CTRL_TYPE_CD: string, PRVDR_NUM: string, NPI: ?int64, RPT_STUS_CD: string, FY_BGN_DT: datetime, FY_END_DT: datetime, PROC_DT: datetime, INITL_RPT_SW: string, LAST_RPT_SW: string, TRNSMTL_NUM: string, FI_NUM: string, ADR_VNDR_CD: string, FI_CREAT_DT: datetime, UTIL_CD: string, NPR_DT: datetime, SPEC_IND: string, FI_RCPT_DT: datetime}</t>
   </si>
 </sst>
 </file>
@@ -192,7 +201,7 @@
     <numFmt numFmtId="165" formatCode="#,##0;\(#,##0\);\-"/>
     <numFmt numFmtId="166" formatCode="0;\(0\);\-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +262,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="14">
@@ -476,7 +492,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="3" fillId="10" borderId="1" xfId="15">
       <protection locked="0"/>
@@ -511,6 +527,9 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="10" borderId="7" xfId="15" applyBorder="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -629,6 +648,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -639,13 +665,6 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -798,7 +817,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F2EFE16-214D-4348-BEF8-975642B9A3BB}" name="Mappings" displayName="Mappings" ref="G3:J10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4" headerRowCellStyle="Шапка_справочник" dataCellStyle="Справочник_данные">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F2EFE16-214D-4348-BEF8-975642B9A3BB}" name="Mappings" displayName="Mappings" ref="G3:J10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4" headerRowCellStyle="Шапка_справочник" dataCellStyle="Справочник_данные">
   <autoFilter ref="G3:J10" xr:uid="{8F2EFE16-214D-4348-BEF8-975642B9A3BB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AFBB63CD-AB05-4E64-9580-DC476A9E2342}" name="DB table" dataDxfId="3" dataCellStyle="Справочник_данные"/>
@@ -1107,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF7D921-30C3-488A-B359-12D8C7E82A3F}">
-  <dimension ref="B2:J11"/>
+  <dimension ref="B2:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1145,7 @@
     <col min="10" max="10" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1137,7 +1156,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1162,7 +1181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1181,11 +1200,14 @@
       <c r="I4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="9" t="s">
         <v>40</v>
       </c>
+      <c r="L4" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1204,11 +1226,14 @@
       <c r="I5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="L5" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1227,11 +1252,14 @@
       <c r="I6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="9" t="s">
         <v>44</v>
       </c>
+      <c r="L6" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1249,7 +1277,7 @@
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1267,7 +1295,7 @@
       </c>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1284,8 +1312,9 @@
         <v>2</v>
       </c>
       <c r="J9" s="3"/>
+      <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>41</v>
       </c>
@@ -1303,7 +1332,7 @@
       </c>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>42</v>
       </c>

</xml_diff>